<commit_message>
few new changes tests
</commit_message>
<xml_diff>
--- a/Models/Prospective_conso/data/Hypotheses_residential_tertiary_BASIC.xlsx
+++ b/Models/Prospective_conso/data/Hypotheses_residential_tertiary_BASIC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://engie-my.sharepoint.com/personal/kv6345_engie_com/Documents/Documents/5-Python/Energy-Alternatives-Planing/Models/Prospective_conso/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="118" documentId="8_{6616B5A7-648E-4099-B71D-DDB13E8D5951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{298AEEF5-CE64-474A-9F7B-E078A02C24EB}"/>
+  <xr:revisionPtr revIDLastSave="138" documentId="8_{6616B5A7-648E-4099-B71D-DDB13E8D5951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6DCBA5B2-11F1-487A-8A01-DB7F2F275568}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0D" sheetId="1" r:id="rId1"/>
@@ -497,12 +497,12 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -510,7 +510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -518,7 +518,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -526,7 +526,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -545,12 +545,12 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -585,7 +585,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -620,7 +620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -655,7 +655,7 @@
         <v>0.72104118463674227</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -690,7 +690,7 @@
         <v>0.56914728682170546</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -725,7 +725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -760,7 +760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -795,7 +795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -830,7 +830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
@@ -865,7 +865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -900,7 +900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -935,7 +935,7 @@
         <v>0.72104118463674227</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -970,7 +970,7 @@
         <v>0.56914728682170546</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1005,7 +1005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1040,7 +1040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -1075,7 +1075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -1110,7 +1110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -1145,7 +1145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
@@ -1180,7 +1180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>9</v>
       </c>
@@ -1215,7 +1215,7 @@
         <v>0.72104118463674227</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>10</v>
       </c>
@@ -1250,7 +1250,7 @@
         <v>0.56914728682170546</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>11</v>
       </c>
@@ -1285,7 +1285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>12</v>
       </c>
@@ -1320,7 +1320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>13</v>
       </c>
@@ -1355,7 +1355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>14</v>
       </c>
@@ -1390,7 +1390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>15</v>
       </c>
@@ -1439,9 +1439,9 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1458,7 +1458,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1475,7 +1475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -1492,7 +1492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -1509,7 +1509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -1526,7 +1526,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -1543,7 +1543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -1560,7 +1560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -1577,7 +1577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -1602,20 +1602,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="26.44140625" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1632,7 +1632,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1648,8 +1648,27 @@
       <c r="E2" s="2">
         <v>66.959052272187947</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" s="2">
+        <v>739982.82830000005</v>
+      </c>
+      <c r="G2">
+        <f>F2*INDEX(retrofit_Transition!$D$2:$D$9,MATCH(res_type_Energy_source!A2,retrofit_Transition!$A$2:$A$9,0))</f>
+        <v>739982.82830000005</v>
+      </c>
+      <c r="H2">
+        <f>F2*INDEX(retrofit_Transition!$F$2:$F$9,MATCH(res_type_Energy_source!A2,retrofit_Transition!$A$2:$A$9,0))</f>
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <f>SUM(G2:G9)</f>
+        <v>1453833.6586302863</v>
+      </c>
+      <c r="J2">
+        <f>SUM(H2:H9)</f>
+        <v>2156906.933220021</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -1665,8 +1684,19 @@
       <c r="E3" s="2">
         <v>68.656688977716797</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3" s="2">
+        <v>1125093.5371900001</v>
+      </c>
+      <c r="G3">
+        <f>F3*INDEX(retrofit_Transition!$D$2:$D$9,MATCH(res_type_Energy_source!A3,retrofit_Transition!$A$2:$A$9,0))</f>
+        <v>42666.087631985421</v>
+      </c>
+      <c r="H3">
+        <f>F3*INDEX(retrofit_Transition!$F$2:$F$9,MATCH(res_type_Energy_source!A3,retrofit_Transition!$A$2:$A$9,0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -1682,8 +1712,19 @@
       <c r="E4" s="2">
         <v>66.283435853153662</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4" s="2">
+        <v>12192189.05123</v>
+      </c>
+      <c r="G4">
+        <f>F4*INDEX(retrofit_Transition!$D$2:$D$9,MATCH(res_type_Energy_source!A4,retrofit_Transition!$A$2:$A$9,0))</f>
+        <v>439698.53886499832</v>
+      </c>
+      <c r="H4">
+        <f>F4*INDEX(retrofit_Transition!$F$2:$F$9,MATCH(res_type_Energy_source!A4,retrofit_Transition!$A$2:$A$9,0))</f>
+        <v>2156906.933220021</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -1699,8 +1740,19 @@
       <c r="E5" s="2">
         <v>52.973740041026069</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5" s="2">
+        <v>7297969.8567000004</v>
+      </c>
+      <c r="G5">
+        <f>F5*INDEX(retrofit_Transition!$D$2:$D$9,MATCH(res_type_Energy_source!A5,retrofit_Transition!$A$2:$A$9,0))</f>
+        <v>231486.20383330251</v>
+      </c>
+      <c r="H5">
+        <f>F5*INDEX(retrofit_Transition!$F$2:$F$9,MATCH(res_type_Energy_source!A5,retrofit_Transition!$A$2:$A$9,0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -1716,8 +1768,19 @@
       <c r="E6" s="2">
         <v>62.634561091350477</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6" s="2">
+        <v>3358242.1158500002</v>
+      </c>
+      <c r="G6">
+        <f>F6*INDEX(retrofit_Transition!$D$2:$D$9,MATCH(res_type_Energy_source!A6,retrofit_Transition!$A$2:$A$9,0))</f>
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <f>F6*INDEX(retrofit_Transition!$F$2:$F$9,MATCH(res_type_Energy_source!A6,retrofit_Transition!$A$2:$A$9,0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -1733,8 +1796,19 @@
       <c r="E7" s="2">
         <v>44.438915275434461</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F7" s="2">
+        <v>975341.69350000005</v>
+      </c>
+      <c r="G7">
+        <f>F7*INDEX(retrofit_Transition!$D$2:$D$9,MATCH(res_type_Energy_source!A7,retrofit_Transition!$A$2:$A$9,0))</f>
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <f>F7*INDEX(retrofit_Transition!$F$2:$F$9,MATCH(res_type_Energy_source!A7,retrofit_Transition!$A$2:$A$9,0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -1750,8 +1824,19 @@
       <c r="E8" s="2">
         <v>10.255134294331031</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F8" s="2">
+        <v>51941.27362</v>
+      </c>
+      <c r="G8">
+        <f>F8*INDEX(retrofit_Transition!$D$2:$D$9,MATCH(res_type_Energy_source!A8,retrofit_Transition!$A$2:$A$9,0))</f>
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <f>F8*INDEX(retrofit_Transition!$F$2:$F$9,MATCH(res_type_Energy_source!A8,retrofit_Transition!$A$2:$A$9,0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -1767,8 +1852,19 @@
       <c r="E9" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F9" s="2">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <f>F9*INDEX(retrofit_Transition!$D$2:$D$9,MATCH(res_type_Energy_source!A9,retrofit_Transition!$A$2:$A$9,0))</f>
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <f>F9*INDEX(retrofit_Transition!$F$2:$F$9,MATCH(res_type_Energy_source!A9,retrofit_Transition!$A$2:$A$9,0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1784,8 +1880,11 @@
       <c r="E10" s="2">
         <v>112.82783563368309</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F10" s="2">
+        <v>14689496.87408</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1801,8 +1900,11 @@
       <c r="E11" s="2">
         <v>116.852067445918</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F11" s="2">
+        <v>9784412.7406500001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1818,8 +1920,11 @@
       <c r="E12" s="2">
         <v>109.2501764322046</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F12" s="2">
+        <v>19472152.805909999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -1835,8 +1940,11 @@
       <c r="E13" s="2">
         <v>105.71703104202599</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F13" s="2">
+        <v>16195642.170980001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -1852,8 +1960,11 @@
       <c r="E14" s="2">
         <v>86.516098080883552</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F14" s="2">
+        <v>39710.88205</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -1869,8 +1980,11 @@
       <c r="E15" s="2">
         <v>92.499838314799049</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F15" s="2">
+        <v>1167117.30259</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -1886,8 +2000,11 @@
       <c r="E16" s="2">
         <v>21.3461165341844</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F16" s="2">
+        <v>62154.175880000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -1903,8 +2020,11 @@
       <c r="E17" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
@@ -1920,8 +2040,11 @@
       <c r="E18" s="2">
         <v>40726800</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F18" s="2">
+        <v>1404372.1673999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>9</v>
       </c>
@@ -1937,8 +2060,11 @@
       <c r="E19" s="2">
         <v>210049200</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F19" s="2">
+        <v>7243074.5913199997</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>10</v>
       </c>
@@ -1954,8 +2080,11 @@
       <c r="E20" s="2">
         <v>501552000</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F20" s="2">
+        <v>17294893.517439999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>14</v>
       </c>
@@ -1971,8 +2100,11 @@
       <c r="E21" s="2">
         <v>204120000</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F21" s="2">
+        <v>7038619.4547699997</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>11</v>
       </c>
@@ -1988,8 +2120,11 @@
       <c r="E22" s="2">
         <v>67748400</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F22" s="2">
+        <v>2336151.31427</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>12</v>
       </c>
@@ -2005,8 +2140,11 @@
       <c r="E23" s="2">
         <v>13996800</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F23" s="2">
+        <v>482648.19118000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>15</v>
       </c>
@@ -2022,8 +2160,11 @@
       <c r="E24" s="2">
         <v>89326800</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F24" s="2">
+        <v>3080233.9423500001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>13</v>
       </c>
@@ -2037,6 +2178,9 @@
         <v>205.31245689655171</v>
       </c>
       <c r="E25" s="2">
+        <v>0</v>
+      </c>
+      <c r="F25" s="2">
         <v>0</v>
       </c>
     </row>
@@ -2052,12 +2196,15 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -2071,7 +2218,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -2085,7 +2232,7 @@
         <v>739982.82830000005</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -2099,7 +2246,7 @@
         <v>1125093.5371900001</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -2113,7 +2260,7 @@
         <v>12192189.05123</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -2127,7 +2274,7 @@
         <v>7297969.8567000004</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -2141,7 +2288,7 @@
         <v>3358242.1158500002</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -2155,7 +2302,7 @@
         <v>975341.69350000005</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -2169,7 +2316,7 @@
         <v>51941.27362</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -2183,7 +2330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -2197,7 +2344,7 @@
         <v>14689496.87408</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -2211,7 +2358,7 @@
         <v>9784412.7406500001</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -2225,7 +2372,7 @@
         <v>19472152.805909999</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -2239,7 +2386,7 @@
         <v>16195642.170980001</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -2253,7 +2400,7 @@
         <v>39710.88205</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -2267,7 +2414,7 @@
         <v>1167117.30259</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -2281,7 +2428,7 @@
         <v>62154.175880000003</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -2295,7 +2442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
@@ -2309,7 +2456,7 @@
         <v>1404372.1673999999</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>9</v>
       </c>
@@ -2323,7 +2470,7 @@
         <v>7243074.5913199997</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>10</v>
       </c>
@@ -2337,7 +2484,7 @@
         <v>17294893.517439999</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>14</v>
       </c>
@@ -2351,7 +2498,7 @@
         <v>7038619.4547699997</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>11</v>
       </c>
@@ -2365,7 +2512,7 @@
         <v>2336151.31427</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>12</v>
       </c>
@@ -2379,7 +2526,7 @@
         <v>482648.19118000002</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>15</v>
       </c>
@@ -2393,7 +2540,7 @@
         <v>3080233.9423500001</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>13</v>
       </c>
@@ -2420,9 +2567,9 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>26</v>
       </c>
@@ -2433,7 +2580,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>21</v>
       </c>
@@ -2444,7 +2591,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
@@ -2455,7 +2602,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
@@ -2466,7 +2613,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>22</v>
       </c>
@@ -2477,7 +2624,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>25</v>
       </c>
@@ -2488,7 +2635,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
Bug resolve heat pump
</commit_message>
<xml_diff>
--- a/Models/Prospective_conso/data/Hypotheses_residential_tertiary_BASIC.xlsx
+++ b/Models/Prospective_conso/data/Hypotheses_residential_tertiary_BASIC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://engie-my.sharepoint.com/personal/kv6345_engie_com/Documents/Documents/5-Python/Energy-Alternatives-Planing/Models/Prospective_conso/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:1_{6BD13914-5E1C-BB4C-A433-75660AC0694F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E127A68-5A55-4C82-A241-C1199D76EEC0}"/>
+  <xr:revisionPtr revIDLastSave="68" documentId="13_ncr:1_{6BD13914-5E1C-BB4C-A433-75660AC0694F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{97C80755-D259-439E-8495-69F6150FF9E1}"/>
   <bookViews>
-    <workbookView xWindow="45972" yWindow="6276" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0D" sheetId="1" r:id="rId1"/>
@@ -1672,7 +1672,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1886,10 +1886,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1898,9 +1898,10 @@
     <col min="4" max="4" width="26.44140625" customWidth="1"/>
     <col min="5" max="5" width="20.33203125" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1917,7 +1918,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1933,12 +1934,8 @@
       <c r="E2" s="2">
         <v>66.959052272187947</v>
       </c>
-      <c r="F2">
-        <f>C2*D2*E2/10^9*0.65</f>
-        <v>2.2421818852866333</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -1954,12 +1951,8 @@
       <c r="E3" s="2">
         <v>68.656688977716797</v>
       </c>
-      <c r="F3">
-        <f t="shared" ref="F3:F25" si="0">C3*D3*E3/10^9*0.65</f>
-        <v>3.7962036108186807</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -1975,12 +1968,8 @@
       <c r="E4" s="2">
         <v>66.283435853153662</v>
       </c>
-      <c r="F4">
-        <f t="shared" si="0"/>
-        <v>34.058378587204011</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -1996,12 +1985,8 @@
       <c r="E5" s="2">
         <v>52.973740041026069</v>
       </c>
-      <c r="F5">
-        <f t="shared" si="0"/>
-        <v>23.041439940051031</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -2017,12 +2002,8 @@
       <c r="E6" s="2">
         <v>62.634561091350477</v>
       </c>
-      <c r="F6">
-        <f t="shared" si="0"/>
-        <v>11.811470666818641</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -2038,12 +2019,8 @@
       <c r="E7" s="2">
         <v>44.438915275434461</v>
       </c>
-      <c r="F7">
-        <f t="shared" si="0"/>
-        <v>2.7049875918968902</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -2059,12 +2036,8 @@
       <c r="E8" s="2">
         <v>10.255134294331031</v>
       </c>
-      <c r="F8">
-        <f t="shared" si="0"/>
-        <v>3.3242906227226227E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -2080,12 +2053,8 @@
       <c r="E9" s="2">
         <v>0</v>
       </c>
-      <c r="F9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -2101,12 +2070,8 @@
       <c r="E10" s="2">
         <v>112.82783563368309</v>
       </c>
-      <c r="F10">
-        <f t="shared" si="0"/>
-        <v>49.416388068948052</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -2122,12 +2087,8 @@
       <c r="E11" s="2">
         <v>116.852067445918</v>
       </c>
-      <c r="F11">
-        <f t="shared" si="0"/>
-        <v>34.917638813062396</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -2143,12 +2104,8 @@
       <c r="E12" s="2">
         <v>109.2501764322046</v>
       </c>
-      <c r="F12">
-        <f t="shared" si="0"/>
-        <v>58.384596506797202</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -2164,12 +2121,8 @@
       <c r="E13" s="2">
         <v>105.71703104202599</v>
       </c>
-      <c r="F13">
-        <f t="shared" si="0"/>
-        <v>56.884145487112882</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -2185,12 +2138,8 @@
       <c r="E14" s="2">
         <v>86.516098080883552</v>
       </c>
-      <c r="F14">
-        <f t="shared" si="0"/>
-        <v>0.13986496717595023</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -2206,12 +2155,8 @@
       <c r="E15" s="2">
         <v>92.499838314799049</v>
       </c>
-      <c r="F15">
-        <f t="shared" si="0"/>
-        <v>3.2253404795534086</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -2227,12 +2172,8 @@
       <c r="E16" s="2">
         <v>21.3461165341844</v>
       </c>
-      <c r="F16">
-        <f t="shared" si="0"/>
-        <v>3.9637775579400104E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -2248,12 +2189,8 @@
       <c r="E17" s="2">
         <v>0</v>
       </c>
-      <c r="F17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
@@ -2269,12 +2206,8 @@
       <c r="E18" s="2">
         <v>40726800</v>
       </c>
-      <c r="F18">
-        <f t="shared" si="0"/>
-        <v>5.4536401062000008</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>9</v>
       </c>
@@ -2290,12 +2223,8 @@
       <c r="E19" s="2">
         <v>210049200</v>
       </c>
-      <c r="F19">
-        <f t="shared" si="0"/>
-        <v>27.313373915100001</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>10</v>
       </c>
@@ -2311,12 +2240,8 @@
       <c r="E20" s="2">
         <v>501552000</v>
       </c>
-      <c r="F20">
-        <f t="shared" si="0"/>
-        <v>64.689461495100005</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>14</v>
       </c>
@@ -2332,12 +2257,8 @@
       <c r="E21" s="2">
         <v>204120000</v>
       </c>
-      <c r="F21">
-        <f t="shared" si="0"/>
-        <v>29.165460866099998</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>11</v>
       </c>
@@ -2353,12 +2274,8 @@
       <c r="E22" s="2">
         <v>67748400</v>
       </c>
-      <c r="F22">
-        <f t="shared" si="0"/>
-        <v>9.0961048386000005</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>12</v>
       </c>
@@ -2374,12 +2291,8 @@
       <c r="E23" s="2">
         <v>13996800</v>
       </c>
-      <c r="F23">
-        <f t="shared" si="0"/>
-        <v>1.9186717212000002</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>15</v>
       </c>
@@ -2395,12 +2308,8 @@
       <c r="E24" s="2">
         <v>89326800</v>
       </c>
-      <c r="F24">
-        <f t="shared" si="0"/>
-        <v>12.8343229677</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>13</v>
       </c>
@@ -2414,10 +2323,6 @@
         <v>0</v>
       </c>
       <c r="E25" s="2">
-        <v>0</v>
-      </c>
-      <c r="F25">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
mise à jour des notebook residentiel_tertiaire
</commit_message>
<xml_diff>
--- a/Models/Prospective_conso/data/Hypotheses_residential_tertiary_BASIC.xlsx
+++ b/Models/Prospective_conso/data/Hypotheses_residential_tertiary_BASIC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://engie-my.sharepoint.com/personal/kv6345_engie_com/Documents/Documents/5-Python/Energy-Alternatives-Planing/Models/Prospective_conso/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robin.girard/Documents/Code/Etude/Energy-Alternatives-Planing/Models/Prospective_conso/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="69" documentId="13_ncr:1_{6BD13914-5E1C-BB4C-A433-75660AC0694F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AC4053BA-81F8-4087-AF3D-43ACE7AC48E5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0451C9B2-202A-914E-B5D0-0F5D050F067D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45972" yWindow="6276" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1860" yWindow="500" windowWidth="28800" windowHeight="16380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0D" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,8 @@
     <sheet name="Energy_source_Vecteur" sheetId="10" r:id="rId4"/>
     <sheet name="res_type_Energy_source" sheetId="4" r:id="rId5"/>
     <sheet name="year_Vecteur" sheetId="8" r:id="rId6"/>
-    <sheet name="res_type_Energy_source_year" sheetId="7" r:id="rId7"/>
-    <sheet name="year_res_type" sheetId="6" r:id="rId8"/>
+    <sheet name="year_res_type" sheetId="6" r:id="rId7"/>
+    <sheet name="year" sheetId="12" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4">res_type_Energy_source!$A$1:$E$1</definedName>
@@ -30,9 +30,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -42,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="41">
   <si>
     <t>Nom</t>
   </si>
@@ -111,9 +109,6 @@
   </si>
   <si>
     <t>building_type</t>
-  </si>
-  <si>
-    <t>retrofit_change_surface</t>
   </si>
   <si>
     <t>direct_emissions</t>
@@ -174,7 +169,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -188,6 +183,19 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -197,7 +205,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -231,22 +239,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -551,18 +576,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="38.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -570,15 +595,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B2">
         <v>0.65283620689655175</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -586,7 +611,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -594,16 +619,8 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="6"/>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -619,21 +636,21 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -665,7 +682,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -697,7 +714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -729,7 +746,7 @@
         <v>0.72104118463674227</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -761,7 +778,7 @@
         <v>0.56914728682170546</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -793,7 +810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -825,7 +842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -857,7 +874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -889,7 +906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
@@ -921,7 +938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -953,7 +970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -985,7 +1002,7 @@
         <v>0.72104118463674227</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1017,7 +1034,7 @@
         <v>0.56914728682170546</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1049,7 +1066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1081,7 +1098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -1113,7 +1130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -1145,7 +1162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -1177,7 +1194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
@@ -1209,7 +1226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>9</v>
       </c>
@@ -1241,7 +1258,7 @@
         <v>0.72104118463674227</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>10</v>
       </c>
@@ -1273,7 +1290,7 @@
         <v>0.56914728682170546</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>11</v>
       </c>
@@ -1305,7 +1322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>12</v>
       </c>
@@ -1337,7 +1354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>13</v>
       </c>
@@ -1369,7 +1386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>14</v>
       </c>
@@ -1401,7 +1418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>15</v>
       </c>
@@ -1447,38 +1464,38 @@
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.77734375" customWidth="1"/>
+    <col min="1" max="1" width="30.83203125" customWidth="1"/>
     <col min="2" max="7" width="24.6640625" customWidth="1"/>
-    <col min="8" max="8" width="18.77734375" customWidth="1"/>
-    <col min="9" max="10" width="8.77734375" customWidth="1"/>
+    <col min="8" max="8" width="18.83203125" customWidth="1"/>
+    <col min="9" max="10" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1494,14 +1511,14 @@
       <c r="E2" s="2">
         <v>1</v>
       </c>
-      <c r="F2" s="5">
-        <v>0</v>
-      </c>
-      <c r="G2" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F2" s="4">
+        <v>0</v>
+      </c>
+      <c r="G2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -1517,14 +1534,14 @@
       <c r="E3" s="2">
         <v>0</v>
       </c>
-      <c r="F3" s="5">
-        <v>0</v>
-      </c>
-      <c r="G3" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F3" s="4">
+        <v>0</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -1540,14 +1557,14 @@
       <c r="E4" s="2">
         <v>0</v>
       </c>
-      <c r="F4" s="5">
-        <v>0</v>
-      </c>
-      <c r="G4" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -1563,14 +1580,14 @@
       <c r="E5" s="2">
         <v>0.23799999999999999</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="4">
         <v>0.248</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -1586,14 +1603,14 @@
       <c r="E6" s="2">
         <v>0</v>
       </c>
-      <c r="F6" s="5">
-        <v>0</v>
-      </c>
-      <c r="G6" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F6" s="4">
+        <v>0</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -1609,14 +1626,14 @@
       <c r="E7" s="2">
         <v>0</v>
       </c>
-      <c r="F7" s="5">
-        <v>0</v>
-      </c>
-      <c r="G7" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F7" s="4">
+        <v>0</v>
+      </c>
+      <c r="G7" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -1632,14 +1649,14 @@
       <c r="E8" s="2">
         <v>0</v>
       </c>
-      <c r="F8" s="5">
-        <v>0</v>
-      </c>
-      <c r="G8" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F8" s="4">
+        <v>0</v>
+      </c>
+      <c r="G8" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -1655,10 +1672,10 @@
       <c r="E9" s="2">
         <v>0</v>
       </c>
-      <c r="F9" s="5">
-        <v>0</v>
-      </c>
-      <c r="G9" s="5">
+      <c r="F9" s="4">
+        <v>0</v>
+      </c>
+      <c r="G9" s="4">
         <v>0</v>
       </c>
     </row>
@@ -1675,61 +1692,61 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.109375" customWidth="1"/>
+    <col min="1" max="1" width="15.1640625" customWidth="1"/>
     <col min="2" max="2" width="14.33203125" customWidth="1"/>
-    <col min="3" max="4" width="20.77734375" customWidth="1"/>
+    <col min="3" max="4" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
         <v>33</v>
       </c>
-      <c r="D1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="4">
+        <v>29</v>
+      </c>
+      <c r="C2" s="3">
         <v>0.85</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
         <v>0.85</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="4">
+        <v>28</v>
+      </c>
+      <c r="C3" s="3">
         <v>0.9</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>0.9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4">
         <v>0.95</v>
@@ -1738,12 +1755,12 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5">
         <v>0.85</v>
@@ -1752,12 +1769,12 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6">
         <v>0.85</v>
@@ -1766,12 +1783,12 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C7">
         <v>0.85</v>
@@ -1780,12 +1797,12 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C8">
         <v>0.85</v>
@@ -1794,12 +1811,12 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C9">
         <v>0.85</v>
@@ -1808,12 +1825,12 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1822,12 +1839,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -1836,12 +1853,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12">
         <v>2.5</v>
@@ -1850,12 +1867,12 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C13">
         <v>3</v>
@@ -1864,12 +1881,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C14">
         <v>0.95</v>
@@ -1888,20 +1905,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.44140625" customWidth="1"/>
+    <col min="4" max="4" width="26.5" customWidth="1"/>
     <col min="5" max="5" width="20.33203125" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1918,7 +1935,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1939,7 +1956,7 @@
         <v>21459505.7855567</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -1956,7 +1973,7 @@
         <v>68.656688977716797</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -1973,7 +1990,7 @@
         <v>66.283435853153662</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -1990,7 +2007,7 @@
         <v>52.973740041026069</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -2007,7 +2024,7 @@
         <v>62.634561091350477</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -2024,7 +2041,7 @@
         <v>44.438915275434461</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -2041,7 +2058,7 @@
         <v>10.255134294331031</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -2058,7 +2075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -2075,7 +2092,7 @@
         <v>112.82783563368309</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -2092,7 +2109,7 @@
         <v>116.852067445918</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -2109,7 +2126,7 @@
         <v>109.2501764322046</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -2126,7 +2143,7 @@
         <v>105.71703104202599</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -2143,7 +2160,7 @@
         <v>86.516098080883552</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -2160,7 +2177,7 @@
         <v>92.499838314799049</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -2177,7 +2194,7 @@
         <v>21.3461165341844</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -2194,7 +2211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
@@ -2211,7 +2228,7 @@
         <v>40726800</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>9</v>
       </c>
@@ -2228,7 +2245,7 @@
         <v>210049200</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>10</v>
       </c>
@@ -2245,7 +2262,7 @@
         <v>501552000</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>14</v>
       </c>
@@ -2262,7 +2279,7 @@
         <v>204120000</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>11</v>
       </c>
@@ -2279,7 +2296,7 @@
         <v>67748400</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>12</v>
       </c>
@@ -2296,7 +2313,7 @@
         <v>13996800</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>15</v>
       </c>
@@ -2313,7 +2330,7 @@
         <v>89326800</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>13</v>
       </c>
@@ -2345,25 +2362,25 @@
       <selection activeCell="B2" sqref="B2:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
       </c>
       <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
         <v>24</v>
       </c>
-      <c r="D1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2">
         <v>2020</v>
@@ -2375,9 +2392,9 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3">
         <v>2020</v>
@@ -2390,9 +2407,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4">
         <v>2020</v>
@@ -2404,9 +2421,9 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5">
         <v>2020</v>
@@ -2418,9 +2435,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6">
         <v>2020</v>
@@ -2432,9 +2449,9 @@
         <v>28.5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7">
         <v>2020</v>
@@ -2453,366 +2470,90 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{167B8BBB-9262-4BF2-B74E-18F4CB92A48B}">
-  <dimension ref="A1:D25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10F7B8F8-3807-4EDB-9473-911A97CF8CDA}">
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="1">
+      <c r="B2" s="2">
         <v>2020</v>
       </c>
-      <c r="D2" s="2">
-        <v>739982.82830000005</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="C2" s="2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="1">
+      <c r="B3" s="2">
+        <v>2050</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="2">
         <v>2020</v>
       </c>
-      <c r="D3" s="2">
-        <v>1125093.5371900001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="1">
+      <c r="C4" s="2">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="2">
+        <v>2050</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="2">
         <v>2020</v>
       </c>
-      <c r="D4" s="2">
-        <v>12192189.05123</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="1">
-        <v>2020</v>
-      </c>
-      <c r="D5" s="2">
-        <v>7297969.8567000004</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="1">
-        <v>2020</v>
-      </c>
-      <c r="D6" s="2">
-        <v>3358242.1158500002</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="1">
-        <v>2020</v>
-      </c>
-      <c r="D7" s="2">
-        <v>975341.69350000005</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="1">
-        <v>2020</v>
-      </c>
-      <c r="D8" s="2">
-        <v>51941.27362</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="1">
-        <v>2020</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="1">
-        <v>2020</v>
-      </c>
-      <c r="D10" s="2">
-        <v>14689496.87408</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="1">
-        <v>2020</v>
-      </c>
-      <c r="D11" s="2">
-        <v>9784412.7406500001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="1">
-        <v>2020</v>
-      </c>
-      <c r="D12" s="2">
-        <v>19472152.805909999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="1">
-        <v>2020</v>
-      </c>
-      <c r="D13" s="2">
-        <v>16195642.170980001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="1">
-        <v>2020</v>
-      </c>
-      <c r="D14" s="2">
-        <v>39710.88205</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="1">
-        <v>2020</v>
-      </c>
-      <c r="D15" s="2">
-        <v>1167117.30259</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="1">
-        <v>2020</v>
-      </c>
-      <c r="D16" s="2">
-        <v>62154.175880000003</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="1">
-        <v>2020</v>
-      </c>
-      <c r="D17" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" s="1" t="s">
+      <c r="C6" s="2">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="1">
-        <v>2020</v>
-      </c>
-      <c r="D18" s="2">
-        <v>1404372.1673999999</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="1">
-        <v>2020</v>
-      </c>
-      <c r="D19" s="2">
-        <v>7243074.5913199997</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="1">
-        <v>2020</v>
-      </c>
-      <c r="D20" s="2">
-        <v>17294893.517439999</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="1">
-        <v>2020</v>
-      </c>
-      <c r="D21" s="2">
-        <v>7038619.4547699997</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="1">
-        <v>2020</v>
-      </c>
-      <c r="D22" s="2">
-        <v>2336151.31427</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" s="1">
-        <v>2020</v>
-      </c>
-      <c r="D23" s="2">
-        <v>482648.19118000002</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="1">
-        <v>2020</v>
-      </c>
-      <c r="D24" s="2">
-        <v>3080233.9423500001</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C25" s="1">
-        <v>2020</v>
-      </c>
-      <c r="D25" s="2">
-        <v>0</v>
+      <c r="B7" s="2">
+        <v>2050</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.3</v>
       </c>
     </row>
   </sheetData>
@@ -2822,94 +2563,91 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10F7B8F8-3807-4EDB-9473-911A97CF8CDA}">
-  <dimension ref="A1:C7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6E4D7B8-7F8A-6D47-8E14-1AE459D21508}">
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="2">
+      <c r="B1" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="6">
         <v>2020</v>
       </c>
-      <c r="C2" s="2">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="2">
+      <c r="B2" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="6">
+        <v>2022</v>
+      </c>
+      <c r="B3" s="8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="6">
+        <v>2025</v>
+      </c>
+      <c r="B4" s="8">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="6">
+        <v>2030</v>
+      </c>
+      <c r="B5" s="8">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="6">
+        <v>2035</v>
+      </c>
+      <c r="B6" s="8">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="6">
+        <v>2040</v>
+      </c>
+      <c r="B7" s="8">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="6">
+        <v>2045</v>
+      </c>
+      <c r="B8" s="8">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="6">
         <v>2050</v>
       </c>
-      <c r="C3" s="2">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="2">
-        <v>2020</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="2">
-        <v>2050</v>
-      </c>
-      <c r="C5" s="2">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="2">
-        <v>2020</v>
-      </c>
-      <c r="C6" s="2">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="2">
-        <v>2050</v>
-      </c>
-      <c r="C7" s="2">
-        <v>0.3</v>
+      <c r="B9" s="8">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
In notebook: new graphs with surfaces and 2 input datasets. Same in py script
</commit_message>
<xml_diff>
--- a/Models/Prospective_conso/data/Hypotheses_residential_tertiary_BASIC.xlsx
+++ b/Models/Prospective_conso/data/Hypotheses_residential_tertiary_BASIC.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://engie-my.sharepoint.com/personal/kv6345_engie_com/Documents/Documents/5-Python/Energy-Alternatives-Planing/Models/Prospective_conso/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="68" documentId="13_ncr:1_{84CDF3A1-E40C-9844-B681-EAA1EDD5B030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E66A786F-D87B-4892-996B-D7A8CB553009}"/>
+  <xr:revisionPtr revIDLastSave="73" documentId="13_ncr:1_{84CDF3A1-E40C-9844-B681-EAA1EDD5B030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9B67021-7812-4693-AEBD-8F72D187A8E1}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0D" sheetId="1" r:id="rId1"/>
     <sheet name="retrofit_Transition" sheetId="2" r:id="rId2"/>
-    <sheet name="Energy_source" sheetId="11" r:id="rId3"/>
+    <sheet name="Energy_source_year" sheetId="11" r:id="rId3"/>
     <sheet name="Energy_source_Vecteur" sheetId="10" r:id="rId4"/>
     <sheet name="res_type_Energy_source" sheetId="4" r:id="rId5"/>
     <sheet name="year_Vecteur" sheetId="8" r:id="rId6"/>
@@ -606,12 +606,12 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -619,7 +619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>40</v>
       </c>
@@ -627,7 +627,7 @@
         <v>0.65283620689655175</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -635,7 +635,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -643,7 +643,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
     </row>
   </sheetData>
@@ -660,21 +660,21 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -706,7 +706,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -738,7 +738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -770,7 +770,7 @@
         <v>0.72104118463674227</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -802,7 +802,7 @@
         <v>0.56914728682170546</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -834,7 +834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -866,7 +866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -898,7 +898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -930,7 +930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
@@ -962,7 +962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -994,7 +994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1026,7 +1026,7 @@
         <v>0.72104118463674227</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1058,7 +1058,7 @@
         <v>0.56914728682170546</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1090,7 +1090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1122,7 +1122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -1154,7 +1154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -1186,7 +1186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -1218,7 +1218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
@@ -1250,7 +1250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>9</v>
       </c>
@@ -1282,7 +1282,7 @@
         <v>0.72104118463674227</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>10</v>
       </c>
@@ -1314,7 +1314,7 @@
         <v>0.56914728682170546</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>11</v>
       </c>
@@ -1346,7 +1346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>12</v>
       </c>
@@ -1378,7 +1378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>13</v>
       </c>
@@ -1410,7 +1410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>14</v>
       </c>
@@ -1442,7 +1442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>15</v>
       </c>
@@ -1485,18 +1485,18 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.85546875" customWidth="1"/>
-    <col min="2" max="7" width="24.7109375" customWidth="1"/>
-    <col min="8" max="8" width="18.85546875" customWidth="1"/>
-    <col min="9" max="9" width="8.85546875" customWidth="1"/>
+    <col min="1" max="1" width="30.88671875" customWidth="1"/>
+    <col min="2" max="7" width="24.6640625" customWidth="1"/>
+    <col min="8" max="8" width="18.88671875" customWidth="1"/>
+    <col min="9" max="9" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1522,7 +1522,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1548,7 +1548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -1574,7 +1574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -1600,7 +1600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -1627,7 +1627,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -1653,7 +1653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -1679,7 +1679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -1705,7 +1705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -1741,17 +1741,17 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
-    <col min="3" max="4" width="20.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="3" max="4" width="20.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1768,7 +1768,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1785,7 +1785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -1802,7 +1802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -1819,7 +1819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -1836,7 +1836,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -1853,7 +1853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -1870,7 +1870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -1887,7 +1887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -1904,7 +1904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -1921,7 +1921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -1938,7 +1938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -1955,7 +1955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -1972,7 +1972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -1989,7 +1989,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -2017,19 +2017,19 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D2" sqref="D2:D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.44140625" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -2046,7 +2046,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -2063,7 +2063,7 @@
         <v>66.959052272187947</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -2080,7 +2080,7 @@
         <v>68.656688977716797</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -2097,7 +2097,7 @@
         <v>66.283435853153662</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -2108,13 +2108,13 @@
         <v>3995209</v>
       </c>
       <c r="D5" s="2">
-        <v>167.49279128952941</v>
+        <v>72.82295273457801</v>
       </c>
       <c r="E5" s="2">
         <v>52.973740041026069</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -2131,7 +2131,7 @@
         <v>62.634561091350477</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -2142,13 +2142,13 @@
         <v>636489.75</v>
       </c>
       <c r="D7" s="2">
-        <v>147.12858456177321</v>
+        <v>63.968949809466615</v>
       </c>
       <c r="E7" s="2">
         <v>44.438915275434461</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -2159,13 +2159,13 @@
         <v>146882.25</v>
       </c>
       <c r="D8" s="2">
-        <v>33.952750283486118</v>
+        <v>14.762065340646139</v>
       </c>
       <c r="E8" s="2">
         <v>10.255134294331031</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -2182,7 +2182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -2199,7 +2199,7 @@
         <v>112.82783563368309</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -2216,7 +2216,7 @@
         <v>116.852067445918</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -2233,7 +2233,7 @@
         <v>109.2501764322046</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -2244,13 +2244,13 @@
         <v>4442744</v>
       </c>
       <c r="D13" s="2">
-        <v>186.3295070204899</v>
+        <v>81.012829139343438</v>
       </c>
       <c r="E13" s="2">
         <v>105.71703104202599</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -2267,7 +2267,7 @@
         <v>86.516098080883552</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -2278,13 +2278,13 @@
         <v>365907.75</v>
       </c>
       <c r="D15" s="2">
-        <v>146.6052858044018</v>
+        <v>63.741428610609482</v>
       </c>
       <c r="E15" s="2">
         <v>92.499838314799049</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -2295,13 +2295,13 @@
         <v>84440.25</v>
       </c>
       <c r="D16" s="2">
-        <v>33.831989031785021</v>
+        <v>14.709560448602184</v>
       </c>
       <c r="E16" s="2">
         <v>21.3461165341844</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -2318,7 +2318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
@@ -2335,7 +2335,7 @@
         <v>40726800</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>9</v>
       </c>
@@ -2352,7 +2352,7 @@
         <v>210049200</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>10</v>
       </c>
@@ -2369,7 +2369,7 @@
         <v>501552000</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>14</v>
       </c>
@@ -2380,13 +2380,13 @@
         <v>1</v>
       </c>
       <c r="D21" s="2">
-        <v>219.82137857142857</v>
+        <v>95.574512422360257</v>
       </c>
       <c r="E21" s="2">
         <v>204120000</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>11</v>
       </c>
@@ -2403,7 +2403,7 @@
         <v>67748400</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>12</v>
       </c>
@@ -2414,13 +2414,13 @@
         <v>1</v>
       </c>
       <c r="D23" s="2">
-        <v>210.89125000000001</v>
+        <v>91.69184782608697</v>
       </c>
       <c r="E23" s="2">
         <v>13996800</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>15</v>
       </c>
@@ -2431,13 +2431,13 @@
         <v>1</v>
       </c>
       <c r="D24" s="2">
-        <v>221.04354189336235</v>
+        <v>96.105887779722764</v>
       </c>
       <c r="E24" s="2">
         <v>89326800</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>13</v>
       </c>
@@ -2469,9 +2469,9 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -2485,7 +2485,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -2499,7 +2499,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -2514,7 +2514,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -2528,7 +2528,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -2542,7 +2542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -2556,7 +2556,7 @@
         <v>28.5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -2570,7 +2570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -2598,9 +2598,9 @@
       <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>22</v>
       </c>
@@ -2611,7 +2611,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
@@ -2622,7 +2622,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
@@ -2633,7 +2633,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
@@ -2644,7 +2644,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
@@ -2655,7 +2655,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
@@ -2666,7 +2666,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -2691,12 +2691,12 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>7</v>
       </c>
@@ -2707,7 +2707,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>2020</v>
       </c>
@@ -2718,7 +2718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>2022</v>
       </c>
@@ -2726,7 +2726,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>2025</v>
       </c>
@@ -2734,7 +2734,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>2030</v>
       </c>
@@ -2742,7 +2742,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>2035</v>
       </c>
@@ -2750,7 +2750,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>2040</v>
       </c>
@@ -2758,7 +2758,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>2045</v>
       </c>
@@ -2766,7 +2766,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>2050</v>
       </c>

</xml_diff>